<commit_message>
Add example picture and update test excel file
</commit_message>
<xml_diff>
--- a/testcases/test.xlsx
+++ b/testcases/test.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feliciano\Documents\workspace\utility\Xlsx2Json\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feliciano\Documents\workspace\utility\Xlsx2Json\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="example" sheetId="9" r:id="rId1"/>
-    <sheet name="weaponStuffs" sheetId="1" r:id="rId2"/>
-    <sheet name="skillStuffs" sheetId="2" r:id="rId3"/>
-    <sheet name="essenceStuffs" sheetId="3" r:id="rId4"/>
-    <sheet name="shieldStuffs" sheetId="4" r:id="rId5"/>
-    <sheet name="essenceFragmentStuffs" sheetId="6" r:id="rId6"/>
-    <sheet name="bottleStuffs" sheetId="5" r:id="rId7"/>
-    <sheet name="map" sheetId="7" r:id="rId8"/>
-    <sheet name="monster" sheetId="8" r:id="rId9"/>
+    <sheet name="monsters" sheetId="9" r:id="rId1"/>
+    <sheet name="shields" sheetId="10" r:id="rId2"/>
+    <sheet name="weaponStuffs" sheetId="1" r:id="rId3"/>
+    <sheet name="skillStuffs" sheetId="2" r:id="rId4"/>
+    <sheet name="essenceStuffs" sheetId="3" r:id="rId5"/>
+    <sheet name="shieldStuffs" sheetId="4" r:id="rId6"/>
+    <sheet name="essenceFragmentStuffs" sheetId="6" r:id="rId7"/>
+    <sheet name="bottleStuffs" sheetId="5" r:id="rId8"/>
+    <sheet name="map" sheetId="7" r:id="rId9"/>
+    <sheet name="monster" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="121">
   <si>
     <t>_id</t>
   </si>
@@ -358,9 +359,6 @@
     <t>weapon</t>
   </si>
   <si>
-    <t>flag</t>
-  </si>
-  <si>
     <t>nums</t>
   </si>
   <si>
@@ -388,10 +386,16 @@
     <t>oh god</t>
   </si>
   <si>
-    <t>shiled@shieldStuffs#_id</t>
-  </si>
-  <si>
     <t>a:11,b:"22",c:true</t>
+  </si>
+  <si>
+    <t>$flag</t>
+  </si>
+  <si>
+    <t>shiled@shieldStuffs#$id</t>
+  </si>
+  <si>
+    <t>$id</t>
   </si>
 </sst>
 </file>
@@ -738,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,19 +783,19 @@
         <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -799,36 +803,39 @@
         <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
         <v>114</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
         <v>115</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
       <c r="E4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" t="s">
         <v>117</v>
-      </c>
-      <c r="G4" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +847,216 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" activeCellId="1" sqref="A1:D2 O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -982,7 +1198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -1195,7 +1411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
@@ -1360,7 +1576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1465,7 +1681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1571,7 +1787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1686,7 +1902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1786,166 +2002,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="17" width="14.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <v>100</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix a bug and update the monsters sheet example
</commit_message>
<xml_diff>
--- a/testcases/test.xlsx
+++ b/testcases/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="monsters" sheetId="9" r:id="rId1"/>
@@ -392,10 +392,10 @@
     <t>$flag</t>
   </si>
   <si>
-    <t>shiled@shieldStuffs#$id</t>
-  </si>
-  <si>
     <t>$id</t>
+  </si>
+  <si>
+    <t>shiled@shields#$id</t>
   </si>
 </sst>
 </file>
@@ -742,13 +742,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -792,7 +796,7 @@
         <v>109</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>110</v>
@@ -1013,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" activeCellId="1" sqref="A1:D2 O12"/>
     </sheetView>
   </sheetViews>
@@ -1024,7 +1028,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
1. Support 'Date' type 2. Upgrade dependency version
</commit_message>
<xml_diff>
--- a/testcases/test.xlsx
+++ b/testcases/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feliciano\Documents\workspace\utility\Xlsx2Json\testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Documents/WorkSpace/Java/Xlsx2Json/testcases/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDBDDE7-C4EB-0349-9307-F414AF6AC7E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monsters" sheetId="9" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="123">
   <si>
     <t>_id</t>
   </si>
@@ -396,24 +397,32 @@
   </si>
   <si>
     <t>shiled@shields#$id</t>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -421,8 +430,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -461,8 +477,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -739,24 +755,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:G4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="7" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="7" width="27.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -778,8 +795,11 @@
       <c r="G1" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>106</v>
       </c>
@@ -801,8 +821,11 @@
       <c r="G2" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>123</v>
       </c>
@@ -824,27 +847,31 @@
       <c r="G3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>20190929</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>112</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
       <c r="E4" t="s">
         <v>116</v>
       </c>
       <c r="G4" t="s">
         <v>117</v>
       </c>
+      <c r="H4">
+        <v>20190228</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -852,19 +879,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="17" width="14.7109375" customWidth="1"/>
+    <col min="1" max="17" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -917,7 +944,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
@@ -970,7 +997,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1009,24 +1036,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O12" activeCellId="1" sqref="A1:D2 O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="4" width="15.5703125" customWidth="1"/>
+    <col min="1" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
@@ -1041,7 +1069,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>123</v>
       </c>
@@ -1056,24 +1084,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="13" width="14.85546875" customWidth="1"/>
+    <col min="1" max="13" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1155,7 +1184,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1197,25 +1226,26 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="21" width="12.5703125" customWidth="1"/>
+    <col min="1" max="21" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -1280,7 +1310,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1375,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1411,24 +1441,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16" width="14.28515625" customWidth="1"/>
+    <col min="1" max="16" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -1478,7 +1509,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1576,24 +1607,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -1622,7 +1654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1681,24 +1713,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="9" width="14.28515625" customWidth="1"/>
+    <col min="1" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -1727,7 +1760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1756,7 +1789,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1786,25 +1819,26 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="10" width="14.28515625" customWidth="1"/>
+    <col min="1" max="10" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -1836,7 +1870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1901,27 +1935,28 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -1947,7 +1982,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -1973,7 +2008,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2000,8 +2035,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>